<commit_message>
uploading reports for the remain workflows
</commit_message>
<xml_diff>
--- a/TodoLyPerfTest/task - 10 todoly workflows/tabulated data.xlsx
+++ b/TodoLyPerfTest/task - 10 todoly workflows/tabulated data.xlsx
@@ -4,21 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="01 flow " sheetId="1" r:id="rId1"/>
     <sheet name="02 flow" sheetId="2" r:id="rId2"/>
     <sheet name="03 flow" sheetId="3" r:id="rId3"/>
     <sheet name="04 flow" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="05 flow" sheetId="5" r:id="rId5"/>
+    <sheet name="06 flow" sheetId="6" r:id="rId6"/>
+    <sheet name="07 flow" sheetId="7" r:id="rId7"/>
+    <sheet name="08 flow" sheetId="8" r:id="rId8"/>
+    <sheet name="09 flow" sheetId="9" r:id="rId9"/>
+    <sheet name="10 flow" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="19">
   <si>
     <t># Samples</t>
   </si>
@@ -60,6 +65,21 @@
   </si>
   <si>
     <t>05 flow - create N child items:main flow</t>
+  </si>
+  <si>
+    <t>06 flow - get and delete all items by root item:main flow</t>
+  </si>
+  <si>
+    <t>07 flow - Pospone the item due date:main flow</t>
+  </si>
+  <si>
+    <t>08 flow - delete all project done items:main flow</t>
+  </si>
+  <si>
+    <t>09 flow - update user settings:main flow</t>
+  </si>
+  <si>
+    <t>10 flow - create and delete all projects:main flow</t>
   </si>
 </sst>
 </file>
@@ -142,7 +162,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -218,11 +237,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66345216"/>
-        <c:axId val="66350464"/>
+        <c:axId val="48413696"/>
+        <c:axId val="48435968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66345216"/>
+        <c:axId val="48413696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -231,7 +250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66350464"/>
+        <c:crossAx val="48435968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -239,7 +258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66350464"/>
+        <c:axId val="48435968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -250,14 +269,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66345216"/>
+        <c:crossAx val="48413696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -287,7 +305,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -363,11 +380,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68656512"/>
-        <c:axId val="68932736"/>
+        <c:axId val="49236224"/>
+        <c:axId val="49238016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68656512"/>
+        <c:axId val="49236224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68932736"/>
+        <c:crossAx val="49238016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -384,7 +401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68932736"/>
+        <c:axId val="49238016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -395,14 +412,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68656512"/>
+        <c:crossAx val="49236224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -432,7 +448,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -508,11 +523,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="141858304"/>
-        <c:axId val="141859840"/>
+        <c:axId val="49262592"/>
+        <c:axId val="49264128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="141858304"/>
+        <c:axId val="49262592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141859840"/>
+        <c:crossAx val="49264128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -529,7 +544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141859840"/>
+        <c:axId val="49264128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -540,14 +555,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141858304"/>
+        <c:crossAx val="49262592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -577,7 +591,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -653,11 +666,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64786432"/>
-        <c:axId val="64787968"/>
+        <c:axId val="49620480"/>
+        <c:axId val="49622016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64786432"/>
+        <c:axId val="49620480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64787968"/>
+        <c:crossAx val="49622016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -674,7 +687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64787968"/>
+        <c:axId val="49622016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +698,1021 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64786432"/>
+        <c:crossAx val="49620480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05 flow'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('05 flow'!$C$6,'05 flow'!$C$13,'05 flow'!$C$20,'05 flow'!$C$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('05 flow'!$F$6,'05 flow'!$F$13,'05 flow'!$F$20,'05 flow'!$F$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13065.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13014.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13017.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="56492800"/>
+        <c:axId val="56494720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="56492800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56494720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56494720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56492800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'05 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('05 flow'!$C$6,'05 flow'!$C$13,'05 flow'!$C$20,'05 flow'!$C$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('05 flow'!$E$6,'05 flow'!$E$13,'05 flow'!$E$20,'05 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7787.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23550.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40151.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15416</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="71559808"/>
+        <c:axId val="71930240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="71559808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71930240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71930240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71559808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('06 flow'!$B$6,'06 flow'!$B$13,'06 flow'!$B$20,'06 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('06 flow'!$E$6,'06 flow'!$E$13,'06 flow'!$E$20,'06 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24684.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24672.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24675.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24704.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="50851840"/>
+        <c:axId val="50853376"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50851840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50853376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50853376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50851840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('06 flow'!$B$6,'06 flow'!$B$13,'06 flow'!$B$20,'06 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('06 flow'!$D$6,'06 flow'!$D$13,'06 flow'!$D$20,'06 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12630.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12457</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="149473920"/>
+        <c:axId val="149479808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="149473920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149479808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="149479808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149473920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'07 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('07 flow'!$B$6,'07 flow'!$B$13,'07 flow'!$B$20,'07 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('07 flow'!$E$6,'07 flow'!$E$13,'07 flow'!$E$20,'07 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9213.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9222.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9195.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9194.7999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="146096512"/>
+        <c:axId val="146098048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="146096512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146098048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="146098048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146096512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'07 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('07 flow'!$B$6,'07 flow'!$B$13,'07 flow'!$B$20,'07 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('07 flow'!$D$6,'07 flow'!$D$13,'07 flow'!$D$20,'07 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7015.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6667.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18127.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58926.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="146028800"/>
+        <c:axId val="146034688"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="146028800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146034688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="146034688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146028800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'08 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('08 flow'!$B$6,'08 flow'!$B$13,'08 flow'!$B$20,'08 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('08 flow'!$E$6,'08 flow'!$E$13,'08 flow'!$E$20,'08 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>25388.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25389.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25400.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25395.800000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="143439744"/>
+        <c:axId val="143441280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="143439744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143441280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="143441280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143439744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -722,7 +1749,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -798,11 +1824,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68366336"/>
-        <c:axId val="68367872"/>
+        <c:axId val="48452352"/>
+        <c:axId val="48453888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68366336"/>
+        <c:axId val="48452352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +1837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68367872"/>
+        <c:crossAx val="48453888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -819,7 +1845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68367872"/>
+        <c:axId val="48453888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +1856,731 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68366336"/>
+        <c:crossAx val="48452352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'08 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('08 flow'!$B$6,'08 flow'!$B$13,'08 flow'!$B$20,'08 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('08 flow'!$D$6,'08 flow'!$D$13,'08 flow'!$D$20,'08 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30531.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17587.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30672.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="151510400"/>
+        <c:axId val="163325056"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="151510400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="163325056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="163325056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151510400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'09 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('09 flow'!$B$6,'09 flow'!$B$13,'09 flow'!$B$20,'09 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('09 flow'!$E$6,'09 flow'!$E$13,'09 flow'!$E$20,'09 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5214.1499999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5180.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5175.3999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="72084480"/>
+        <c:axId val="72086272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="72084480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72086272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="72086272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72084480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'09 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('09 flow'!$B$6,'09 flow'!$B$13,'09 flow'!$B$20,'09 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('09 flow'!$D$6,'09 flow'!$D$13,'09 flow'!$D$20,'09 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3690.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4119.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5322.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7101.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="151548288"/>
+        <c:axId val="151549824"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="151548288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151549824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="151549824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151548288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('10 flow'!$B$6,'10 flow'!$B$13,'10 flow'!$B$20,'10 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('10 flow'!$E$6,'10 flow'!$E$13,'10 flow'!$E$20,'10 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28938.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28932.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28845.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28848.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="143581184"/>
+        <c:axId val="143582720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="143581184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143582720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="143582720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="143581184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('10 flow'!$B$6,'10 flow'!$B$13,'10 flow'!$B$20,'10 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('10 flow'!$D$6,'10 flow'!$D$13,'10 flow'!$D$20,'10 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10469</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15529.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="144779520"/>
+        <c:axId val="144781312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="144779520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144781312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="144781312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144779520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -867,7 +2617,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -943,11 +2692,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68768512"/>
-        <c:axId val="68770048"/>
+        <c:axId val="48486656"/>
+        <c:axId val="48955392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68768512"/>
+        <c:axId val="48486656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +2705,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68770048"/>
+        <c:crossAx val="48955392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -964,7 +2713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68770048"/>
+        <c:axId val="48955392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,14 +2724,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68768512"/>
+        <c:crossAx val="48486656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1012,7 +2760,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1088,11 +2835,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="114753920"/>
-        <c:axId val="114755456"/>
+        <c:axId val="48990080"/>
+        <c:axId val="48991616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="114753920"/>
+        <c:axId val="48990080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +2848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114755456"/>
+        <c:crossAx val="48991616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1109,7 +2856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114755456"/>
+        <c:axId val="48991616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,14 +2867,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114753920"/>
+        <c:crossAx val="48990080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1157,7 +2903,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1233,11 +2978,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="160756480"/>
-        <c:axId val="160758016"/>
+        <c:axId val="49026944"/>
+        <c:axId val="49028480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="160756480"/>
+        <c:axId val="49026944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,7 +2991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160758016"/>
+        <c:crossAx val="49028480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1254,7 +2999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160758016"/>
+        <c:axId val="49028480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,14 +3010,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160756480"/>
+        <c:crossAx val="49026944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1302,7 +3046,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1378,11 +3121,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="160640000"/>
-        <c:axId val="160813824"/>
+        <c:axId val="49048960"/>
+        <c:axId val="49058944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="160640000"/>
+        <c:axId val="49048960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,7 +3134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160813824"/>
+        <c:crossAx val="49058944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1399,7 +3142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160813824"/>
+        <c:axId val="49058944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,14 +3153,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160640000"/>
+        <c:crossAx val="49048960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1447,7 +3189,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1523,11 +3264,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="65107840"/>
-        <c:axId val="65109376"/>
+        <c:axId val="49124480"/>
+        <c:axId val="49126016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65107840"/>
+        <c:axId val="49124480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,7 +3277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65109376"/>
+        <c:crossAx val="49126016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1544,7 +3285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65109376"/>
+        <c:axId val="49126016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,14 +3296,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65107840"/>
+        <c:crossAx val="49124480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1592,7 +3332,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1668,11 +3407,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143136640"/>
-        <c:axId val="143138176"/>
+        <c:axId val="49142400"/>
+        <c:axId val="49561984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143136640"/>
+        <c:axId val="49142400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,7 +3420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143138176"/>
+        <c:crossAx val="49561984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1689,7 +3428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143138176"/>
+        <c:axId val="49561984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1700,14 +3439,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143136640"/>
+        <c:crossAx val="49142400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1737,7 +3475,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1813,11 +3550,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147109376"/>
-        <c:axId val="147110912"/>
+        <c:axId val="49590656"/>
+        <c:axId val="49592192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147109376"/>
+        <c:axId val="49590656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +3563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147110912"/>
+        <c:crossAx val="49592192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1834,7 +3571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147110912"/>
+        <c:axId val="49592192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1845,14 +3582,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147109376"/>
+        <c:crossAx val="49590656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1954,6 +3690,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2239,6 +4040,331 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>163606</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>49306</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>174812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>358589</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>60512</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>560294</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>186018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>96370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>172570</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>17929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>94129</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>414617</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>11205</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>186018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>347382</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>62753</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>369795</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>138953</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82923</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>174811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>392206</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>60511</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2801,6 +4927,263 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10222</v>
+      </c>
+      <c r="E4" s="1">
+        <v>28938.2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9652</v>
+      </c>
+      <c r="E5" s="1">
+        <v>28938.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(C4:C5)</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:E6" si="0">AVERAGE(D4:D5)</f>
+        <v>9937</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>28938.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>10795</v>
+      </c>
+      <c r="E11" s="1">
+        <v>28926.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10143</v>
+      </c>
+      <c r="E12" s="1">
+        <v>28939.3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(C11:C12)</f>
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:E13" si="1">AVERAGE(D11:D12)</f>
+        <v>10469</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>28932.75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1">
+        <v>12323</v>
+      </c>
+      <c r="E18" s="1">
+        <v>28889.7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1">
+        <v>18736</v>
+      </c>
+      <c r="E19" s="1">
+        <v>28801.3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(C18:C19)</f>
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:E20" si="2">AVERAGE(D18:D19)</f>
+        <v>15529.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>28845.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <v>13531</v>
+      </c>
+      <c r="E25" s="1">
+        <v>28852</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>17461</v>
+      </c>
+      <c r="E26" s="1">
+        <v>28845.9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C25:C26)</f>
+        <v>100</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" ref="D27:E27" si="3">AVERAGE(D25:D26)</f>
+        <v>15496</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>28848.95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E31"/>
@@ -3587,8 +5970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,7 +5982,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3617,13 +6000,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
-        <v>6708</v>
+        <v>8160</v>
       </c>
       <c r="F4" s="1">
-        <v>8142.5</v>
+        <v>13052.3</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
@@ -3631,34 +6014,34 @@
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
-        <v>6010</v>
+        <v>7415</v>
       </c>
       <c r="F5" s="1">
-        <v>8159.3</v>
+        <v>13077.8</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
         <f>AVERAGE(D4:D5)</f>
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6:F6" si="0">AVERAGE(E4:E5)</f>
-        <v>6359</v>
+        <v>7787.5</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>8150.9</v>
+        <v>13065.05</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -3676,13 +6059,13 @@
         <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1">
-        <v>6708</v>
+        <v>19211</v>
       </c>
       <c r="F11" s="1">
-        <v>8142.5</v>
+        <v>13010.9</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
@@ -3690,34 +6073,34 @@
         <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1">
-        <v>6010</v>
+        <v>27890</v>
       </c>
       <c r="F12" s="1">
-        <v>8159.3</v>
+        <v>13011.1</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1">
         <f>AVERAGE(D11:D12)</f>
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ref="E13" si="1">AVERAGE(E11:E12)</f>
-        <v>6359</v>
+        <v>23550.5</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ref="F13" si="2">AVERAGE(F11:F12)</f>
-        <v>8150.9</v>
+        <v>13011</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -3734,13 +6117,13 @@
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>70</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>8334</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>13016.6</v>
       </c>
     </row>
@@ -3748,19 +6131,19 @@
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>70</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>71969</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>13012.2</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="1">
         <f>AVERAGE(D18:D19)</f>
@@ -3776,7 +6159,7 @@
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -3793,13 +6176,13 @@
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>100</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>8822</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>13020.3</v>
       </c>
     </row>
@@ -3807,13 +6190,13 @@
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>100</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>22010</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>13015</v>
       </c>
     </row>
@@ -3836,5 +6219,1034 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E27"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>11188</v>
+      </c>
+      <c r="E4" s="1">
+        <v>24706</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12182</v>
+      </c>
+      <c r="E5" s="1">
+        <v>24663.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(C4:C5)</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:E6" si="0">AVERAGE(D4:D5)</f>
+        <v>11685</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>24684.75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>12793</v>
+      </c>
+      <c r="E11" s="1">
+        <v>24671.599999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>12468</v>
+      </c>
+      <c r="E12" s="1">
+        <v>24673.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(C11:C12)</f>
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:E13" si="1">AVERAGE(D11:D12)</f>
+        <v>12630.5</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>24672.55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1">
+        <v>29231</v>
+      </c>
+      <c r="E18" s="1">
+        <v>24675.1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1">
+        <v>13413</v>
+      </c>
+      <c r="E19" s="1">
+        <v>24675.3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(C18:C19)</f>
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:E20" si="2">AVERAGE(D18:D19)</f>
+        <v>21322</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>24675.199999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <v>13490</v>
+      </c>
+      <c r="E25" s="1">
+        <v>24686.799999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>11424</v>
+      </c>
+      <c r="E26" s="1">
+        <v>24721.9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C25:C26)</f>
+        <v>100</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" ref="D27:E27" si="3">AVERAGE(D25:D26)</f>
+        <v>12457</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>24704.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6701</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9221.2000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7330</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9205.2000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(C4:C5)</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:E6" si="0">AVERAGE(D4:D5)</f>
+        <v>7015.5</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>9213.2000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5524</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9209.2999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7811</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9235.2000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(C11:C12)</f>
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:E13" si="1">AVERAGE(D11:D12)</f>
+        <v>6667.5</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>9222.25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1">
+        <v>30163</v>
+      </c>
+      <c r="E18" s="1">
+        <v>9194.7000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6092</v>
+      </c>
+      <c r="E19" s="1">
+        <v>9195.7999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(C18:C19)</f>
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:E20" si="2">AVERAGE(D18:D19)</f>
+        <v>18127.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>9195.25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <v>22414</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9194.7999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>95439</v>
+      </c>
+      <c r="E26" s="1">
+        <v>9194.7999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C25:C26)</f>
+        <v>100</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" ref="D27:E27" si="3">AVERAGE(D25:D26)</f>
+        <v>58926.5</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>9194.7999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>13428</v>
+      </c>
+      <c r="E4" s="1">
+        <v>25388.2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>33332</v>
+      </c>
+      <c r="E5" s="1">
+        <v>25388.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(C4:C5)</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:E6" si="0">AVERAGE(D4:D5)</f>
+        <v>23380</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>25388.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>22454</v>
+      </c>
+      <c r="E11" s="1">
+        <v>25389.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>38609</v>
+      </c>
+      <c r="E12" s="1">
+        <v>25389.9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(C11:C12)</f>
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:E13" si="1">AVERAGE(D11:D12)</f>
+        <v>30531.5</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>25389.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1">
+        <v>16050</v>
+      </c>
+      <c r="E18" s="1">
+        <v>25401.3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19125</v>
+      </c>
+      <c r="E19" s="1">
+        <v>25399</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(C18:C19)</f>
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:E20" si="2">AVERAGE(D18:D19)</f>
+        <v>17587.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>25400.15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44404</v>
+      </c>
+      <c r="E25" s="1">
+        <v>25394.2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>16941</v>
+      </c>
+      <c r="E26" s="1">
+        <v>25397.4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C25:C26)</f>
+        <v>100</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" ref="D27:E27" si="3">AVERAGE(D25:D26)</f>
+        <v>30672.5</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>25395.800000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E27"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3986</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5212.8999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3395</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5215.3999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>AVERAGE(C4:C5)</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:E6" si="0">AVERAGE(D4:D5)</f>
+        <v>3690.5</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>5214.1499999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4067</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5199.1000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4172</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5192.8999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f>AVERAGE(C11:C12)</f>
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:E13" si="1">AVERAGE(D11:D12)</f>
+        <v>4119.5</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>5196</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5751</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5173.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4894</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5187.3999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(C18:C19)</f>
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" ref="D20:E20" si="2">AVERAGE(D18:D19)</f>
+        <v>5322.5</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>5180.45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+      <c r="D25" s="1">
+        <v>7832</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5177.1000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>6371</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5173.7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C25:C26)</f>
+        <v>100</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" ref="D27:E27" si="3">AVERAGE(D25:D26)</f>
+        <v>7101.5</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>5175.3999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changing excel extension to .xls
</commit_message>
<xml_diff>
--- a/TodoLyPerfTest/task - 10 todoly workflows/tabulated data.xlsx
+++ b/TodoLyPerfTest/task - 10 todoly workflows/tabulated data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="01 flow " sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="09 flow" sheetId="9" r:id="rId9"/>
     <sheet name="10 flow" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -130,9 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,6 +146,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -150,7 +156,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -162,6 +168,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -237,20 +244,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48413696"/>
-        <c:axId val="48435968"/>
+        <c:axId val="-924618064"/>
+        <c:axId val="-924617520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48413696"/>
+        <c:axId val="-924618064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48435968"/>
+        <c:crossAx val="-924617520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -258,7 +266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48435968"/>
+        <c:axId val="-924617520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,13 +277,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48413696"/>
+        <c:crossAx val="-924618064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -293,436 +302,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'04 flow'!$F$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Avg. Bytes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('04 flow'!$C$6,'04 flow'!$C$13,'04 flow'!$C$20,'04 flow'!$C$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('04 flow'!$F$6,'04 flow'!$F$13,'04 flow'!$F$20,'04 flow'!$F$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12387.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8158.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8138</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8150.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="49236224"/>
-        <c:axId val="49238016"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="49236224"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49238016"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="49238016"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49236224"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'04 flow'!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Response time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('04 flow'!$C$6,'04 flow'!$C$13,'04 flow'!$C$20,'04 flow'!$C$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('04 flow'!$E$6,'04 flow'!$E$13,'04 flow'!$E$20,'04 flow'!$E$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>7646</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5527</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14598</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6359</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="49262592"/>
-        <c:axId val="49264128"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="49262592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49264128"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="49264128"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49262592"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'04 flow'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v># Samples</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('04 flow'!$C$6,'04 flow'!$C$13,'04 flow'!$C$20,'04 flow'!$C$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('04 flow'!$D$6,'04 flow'!$D$13,'04 flow'!$D$20,'04 flow'!$D$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="49620480"/>
-        <c:axId val="49622016"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="49620480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49622016"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="49622016"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49620480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -810,20 +390,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="56492800"/>
-        <c:axId val="56494720"/>
+        <c:axId val="-704555696"/>
+        <c:axId val="-704546448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56492800"/>
+        <c:axId val="-704555696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56494720"/>
+        <c:crossAx val="-704546448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -831,7 +412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56494720"/>
+        <c:axId val="-704546448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56492800"/>
+        <c:crossAx val="-704555696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -864,10 +445,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -955,20 +536,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="71559808"/>
-        <c:axId val="71930240"/>
+        <c:axId val="-704550800"/>
+        <c:axId val="-704544816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71559808"/>
+        <c:axId val="-704550800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71930240"/>
+        <c:crossAx val="-704544816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -976,7 +558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71930240"/>
+        <c:axId val="-704544816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -987,7 +569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71559808"/>
+        <c:crossAx val="-704550800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1009,10 +591,1162 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('06 flow'!$B$6,'06 flow'!$B$13,'06 flow'!$B$20,'06 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('06 flow'!$E$6,'06 flow'!$E$13,'06 flow'!$E$20,'06 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24684.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24672.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24675.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24704.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704545904"/>
+        <c:axId val="-704545360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704545904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704545360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704545360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704545904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('06 flow'!$B$6,'06 flow'!$B$13,'06 flow'!$B$20,'06 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('06 flow'!$D$6,'06 flow'!$D$13,'06 flow'!$D$20,'06 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12630.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12457</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704888560"/>
+        <c:axId val="-704899440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704888560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704899440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704899440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704888560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'07 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('07 flow'!$B$6,'07 flow'!$B$13,'07 flow'!$B$20,'07 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('07 flow'!$E$6,'07 flow'!$E$13,'07 flow'!$E$20,'07 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9213.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9222.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9195.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9194.7999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704889648"/>
+        <c:axId val="-704887472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704889648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704887472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704887472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704889648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'07 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('07 flow'!$B$6,'07 flow'!$B$13,'07 flow'!$B$20,'07 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('07 flow'!$D$6,'07 flow'!$D$13,'07 flow'!$D$20,'07 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7015.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6667.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18127.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58926.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704901072"/>
+        <c:axId val="-704895088"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704901072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704895088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704895088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704901072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'08 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('08 flow'!$B$6,'08 flow'!$B$13,'08 flow'!$B$20,'08 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('08 flow'!$E$6,'08 flow'!$E$13,'08 flow'!$E$20,'08 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>25388.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25389.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25400.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25395.800000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704891280"/>
+        <c:axId val="-704886384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704891280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704886384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704886384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704891280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'08 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('08 flow'!$B$6,'08 flow'!$B$13,'08 flow'!$B$20,'08 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('08 flow'!$D$6,'08 flow'!$D$13,'08 flow'!$D$20,'08 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30531.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17587.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30672.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704892368"/>
+        <c:axId val="-704898896"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704892368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704898896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704898896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704892368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'09 flow'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('09 flow'!$B$6,'09 flow'!$B$13,'09 flow'!$B$20,'09 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('09 flow'!$E$6,'09 flow'!$E$13,'09 flow'!$E$20,'09 flow'!$E$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5214.1499999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5180.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5175.3999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704893456"/>
+        <c:axId val="-704892912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704893456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704892912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704892912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704893456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'09 flow'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Response time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('09 flow'!$B$6,'09 flow'!$B$13,'09 flow'!$B$20,'09 flow'!$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('09 flow'!$D$6,'09 flow'!$D$13,'09 flow'!$D$20,'09 flow'!$D$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3690.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4119.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5322.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7101.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704901616"/>
+        <c:axId val="-704895632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704901616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704895632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704895632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704901616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1038,18 +1772,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'06 flow'!$E$3</c:f>
+              <c:f>'01 flow '!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Avg. Bytes</c:v>
+                  <c:v>Response time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>('06 flow'!$B$6,'06 flow'!$B$13,'06 flow'!$B$20,'06 flow'!$B$27)</c:f>
+              <c:f>('01 flow '!$B$6,'01 flow '!$B$15,'01 flow '!$B$24,'01 flow '!$B$32)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1069,21 +1803,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('06 flow'!$E$6,'06 flow'!$E$13,'06 flow'!$E$20,'06 flow'!$E$27)</c:f>
+              <c:f>('01 flow '!$D$6,'01 flow '!$D$15,'01 flow '!$D$24,'01 flow '!$D$32)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>24684.75</c:v>
+                  <c:v>2704.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24672.55</c:v>
+                  <c:v>2898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24675.199999999997</c:v>
+                  <c:v>3784.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24704.35</c:v>
+                  <c:v>3961.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,20 +1834,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50851840"/>
-        <c:axId val="50853376"/>
+        <c:axId val="-704991328"/>
+        <c:axId val="-704986432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50851840"/>
+        <c:axId val="-704991328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50853376"/>
+        <c:crossAx val="-704986432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1121,7 +1856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50853376"/>
+        <c:axId val="-704986432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1867,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50851840"/>
+        <c:crossAx val="-704991328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1154,1168 +1889,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'06 flow'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Response time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('06 flow'!$B$6,'06 flow'!$B$13,'06 flow'!$B$20,'06 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('06 flow'!$D$6,'06 flow'!$D$13,'06 flow'!$D$20,'06 flow'!$D$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>11685</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12630.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21322</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12457</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="149473920"/>
-        <c:axId val="149479808"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="149473920"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149479808"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="149479808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149473920"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'07 flow'!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Avg. Bytes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('07 flow'!$B$6,'07 flow'!$B$13,'07 flow'!$B$20,'07 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('07 flow'!$E$6,'07 flow'!$E$13,'07 flow'!$E$20,'07 flow'!$E$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>9213.2000000000007</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9222.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9195.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9194.7999999999993</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="146096512"/>
-        <c:axId val="146098048"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="146096512"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146098048"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="146098048"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146096512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'07 flow'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Response time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('07 flow'!$B$6,'07 flow'!$B$13,'07 flow'!$B$20,'07 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('07 flow'!$D$6,'07 flow'!$D$13,'07 flow'!$D$20,'07 flow'!$D$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>7015.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6667.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18127.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58926.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="146028800"/>
-        <c:axId val="146034688"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="146028800"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146034688"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="146034688"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146028800"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'08 flow'!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Avg. Bytes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('08 flow'!$B$6,'08 flow'!$B$13,'08 flow'!$B$20,'08 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('08 flow'!$E$6,'08 flow'!$E$13,'08 flow'!$E$20,'08 flow'!$E$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>25388.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25389.7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25400.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25395.800000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="143439744"/>
-        <c:axId val="143441280"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="143439744"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143441280"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="143441280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143439744"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'01 flow '!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Response time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('01 flow '!$B$6,'01 flow '!$B$15,'01 flow '!$B$24,'01 flow '!$B$32)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('01 flow '!$D$6,'01 flow '!$D$15,'01 flow '!$D$24,'01 flow '!$D$32)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2704.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2898</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3784.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3961.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="48452352"/>
-        <c:axId val="48453888"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="48452352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48453888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="48453888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48452352"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'08 flow'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Response time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('08 flow'!$B$6,'08 flow'!$B$13,'08 flow'!$B$20,'08 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('08 flow'!$D$6,'08 flow'!$D$13,'08 flow'!$D$20,'08 flow'!$D$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>23380</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30531.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17587.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30672.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="151510400"/>
-        <c:axId val="163325056"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="151510400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163325056"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="163325056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151510400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'09 flow'!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Avg. Bytes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('09 flow'!$B$6,'09 flow'!$B$13,'09 flow'!$B$20,'09 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('09 flow'!$E$6,'09 flow'!$E$13,'09 flow'!$E$20,'09 flow'!$E$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5214.1499999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5196</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5180.45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5175.3999999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="72084480"/>
-        <c:axId val="72086272"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="72084480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72086272"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="72086272"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72084480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'09 flow'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Response time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('09 flow'!$B$6,'09 flow'!$B$13,'09 flow'!$B$20,'09 flow'!$B$27)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('09 flow'!$D$6,'09 flow'!$D$13,'09 flow'!$D$20,'09 flow'!$D$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3690.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4119.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5322.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7101.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="151548288"/>
-        <c:axId val="151549824"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="151548288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151549824"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="151549824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151548288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2403,20 +1980,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143581184"/>
-        <c:axId val="143582720"/>
+        <c:axId val="-704891824"/>
+        <c:axId val="-703511984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143581184"/>
+        <c:axId val="-704891824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143582720"/>
+        <c:crossAx val="-703511984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2424,7 +2002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143582720"/>
+        <c:axId val="-703511984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,7 +2013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143581184"/>
+        <c:crossAx val="-704891824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2457,10 +2035,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2548,20 +2126,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144779520"/>
-        <c:axId val="144781312"/>
+        <c:axId val="-703519056"/>
+        <c:axId val="-703513072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144779520"/>
+        <c:axId val="-703519056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144781312"/>
+        <c:crossAx val="-703513072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2569,7 +2148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144781312"/>
+        <c:axId val="-703513072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144779520"/>
+        <c:crossAx val="-703519056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2605,7 +2184,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2617,6 +2196,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2692,20 +2272,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48486656"/>
-        <c:axId val="48955392"/>
+        <c:axId val="-704997856"/>
+        <c:axId val="-704997312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48486656"/>
+        <c:axId val="-704997856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48955392"/>
+        <c:crossAx val="-704997312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2713,7 +2294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48955392"/>
+        <c:axId val="-704997312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2724,13 +2305,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48486656"/>
+        <c:crossAx val="-704997856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2748,7 +2330,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2760,6 +2342,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2835,20 +2418,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48990080"/>
-        <c:axId val="48991616"/>
+        <c:axId val="-704992416"/>
+        <c:axId val="-704989696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48990080"/>
+        <c:axId val="-704992416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48991616"/>
+        <c:crossAx val="-704989696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2856,7 +2440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48991616"/>
+        <c:axId val="-704989696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2867,13 +2451,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48990080"/>
+        <c:crossAx val="-704992416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2891,7 +2476,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2903,6 +2488,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2978,20 +2564,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49026944"/>
-        <c:axId val="49028480"/>
+        <c:axId val="-704987520"/>
+        <c:axId val="-704995136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49026944"/>
+        <c:axId val="-704987520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49028480"/>
+        <c:crossAx val="-704995136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2999,7 +2586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49028480"/>
+        <c:axId val="-704995136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3010,13 +2597,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49026944"/>
+        <c:crossAx val="-704987520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3034,7 +2622,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3046,149 +2634,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'02 flow'!$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v># Samples</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>('02 flow'!$B$7,'02 flow'!$B$15,'02 flow'!$B$23,'02 flow'!$B$31)</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Total 10 users</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Total 40 users</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Total 70 users</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Total 100 users</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>('02 flow'!$C$7,'02 flow'!$C$15,'02 flow'!$C$23,'02 flow'!$C$31)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="49048960"/>
-        <c:axId val="49058944"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="49048960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49058944"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="49058944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49048960"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3264,20 +2710,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49124480"/>
-        <c:axId val="49126016"/>
+        <c:axId val="-704994048"/>
+        <c:axId val="-704988608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49124480"/>
+        <c:axId val="-704994048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49126016"/>
+        <c:crossAx val="-704988608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3285,7 +2732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49126016"/>
+        <c:axId val="-704988608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,13 +2743,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49124480"/>
+        <c:crossAx val="-704994048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3317,10 +2765,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3332,6 +2780,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3407,20 +2856,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49142400"/>
-        <c:axId val="49561984"/>
+        <c:axId val="-704988064"/>
+        <c:axId val="-704999488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49142400"/>
+        <c:axId val="-704988064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49561984"/>
+        <c:crossAx val="-704999488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3428,7 +2878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49561984"/>
+        <c:axId val="-704999488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3439,13 +2889,160 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49142400"/>
+        <c:crossAx val="-704988064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'04 flow'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg. Bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>('04 flow'!$C$6,'04 flow'!$C$13,'04 flow'!$C$20,'04 flow'!$C$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Total 10 users</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total 40 users</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Total 70 users</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total 100 users</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('04 flow'!$F$6,'04 flow'!$F$13,'04 flow'!$F$20,'04 flow'!$F$27)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12387.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8158.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8150.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-704552432"/>
+        <c:axId val="-704542640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-704552432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704542640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-704542640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-704552432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3463,7 +3060,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3475,6 +3072,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3488,18 +3086,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'03 flow'!$C$3</c:f>
+              <c:f>'04 flow'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v># Samples</c:v>
+                  <c:v>Response time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>('03 flow'!$B$6,'03 flow'!$B$13,'03 flow'!$B$20,'03 flow'!$B$27)</c:f>
+              <c:f>('04 flow'!$C$6,'04 flow'!$C$13,'04 flow'!$C$20,'04 flow'!$C$27)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -3519,21 +3117,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('03 flow'!$C$6,'03 flow'!$C$13,'03 flow'!$C$20,'03 flow'!$C$27)</c:f>
+              <c:f>('04 flow'!$E$6,'04 flow'!$E$13,'04 flow'!$E$20,'04 flow'!$E$27)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>7646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>5527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>14598</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>6359</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3550,20 +3148,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49590656"/>
-        <c:axId val="49592192"/>
+        <c:axId val="-704549712"/>
+        <c:axId val="-704543184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49590656"/>
+        <c:axId val="-704549712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49592192"/>
+        <c:crossAx val="-704543184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3571,7 +3170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49592192"/>
+        <c:axId val="-704543184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,13 +3181,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49590656"/>
+        <c:crossAx val="-704549712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3693,6 +3293,319 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11228295" y="190500"/>
+          <a:ext cx="3597088" cy="1400735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100"/>
+            <a:t>The average of the bytes</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0"/>
+            <a:t> sent </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>shows an decrease </a:t>
+          </a:r>
+          <a:endParaRPr lang="es-BO">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100"/>
+            <a:t>as the number of the user</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0"/>
+            <a:t> grows .</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0"/>
+            <a:t>it should be needed to take more samples in order to verify this behavior</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-BO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CuadroTexto 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10230971" y="3182471"/>
+          <a:ext cx="3585882" cy="1557617"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The average of response</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> time shows an increase on its value </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>as the number of the user</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> grows meaning . </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>take in account the endpoints requires more mandatory parameters in its body.</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-BO">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CuadroTexto 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11273118" y="6824382"/>
+          <a:ext cx="3036794" cy="1243853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-BO" sz="1100" baseline="0"/>
+            <a:t> counter shows the relation between number of samples and number of users its values increases along the each test executions for every workflow </a:t>
+          </a:r>
+          <a:endParaRPr lang="es-BO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3825,36 +3738,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3920,36 +3803,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>17929</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>336176</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>94129</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4010,36 +3863,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4374,7 +4197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4416,7 +4239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4451,7 +4274,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4662,13 +4485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="B2:E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
@@ -4676,8 +4499,8 @@
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -4738,8 +4561,8 @@
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -4800,8 +4623,8 @@
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -4862,8 +4685,8 @@
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -4931,11 +4754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -5188,13 +5011,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:E31"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5202,8 +5025,8 @@
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -5264,8 +5087,8 @@
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -5388,8 +5211,8 @@
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -5458,18 +5281,18 @@
   <dimension ref="B3:E27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -5527,8 +5350,8 @@
         <v>16637.45</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -5586,8 +5409,8 @@
         <v>16639.45</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -5645,8 +5468,8 @@
         <v>16598.400000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -5714,11 +5537,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
@@ -5971,10 +5794,10 @@
   <dimension ref="C3:F27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:F27"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -6231,7 +6054,7 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -6488,7 +6311,7 @@
       <selection activeCell="B24" sqref="B24:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
@@ -6745,7 +6568,7 @@
       <selection activeCell="B24" sqref="B24:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
@@ -7002,7 +6825,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>

</xml_diff>